<commit_message>
Associado produto novo ao grupo
</commit_message>
<xml_diff>
--- a/Documentação/Horas Trabalhadas.xlsx
+++ b/Documentação/Horas Trabalhadas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Quantidade de horas trabalhadas no Projeto</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Criando Repositores, Services, DTO, Controllers</t>
+  </si>
+  <si>
+    <t>Procurando solução para assossiar Produtos com Grupos</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,16 +548,22 @@
         <v>44229</v>
       </c>
       <c r="B13" s="5">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
+      <c r="A14" s="4">
+        <v>44230</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>

</xml_diff>

<commit_message>
Associação Pedido Cliete Ok
</commit_message>
<xml_diff>
--- a/Documentação/Horas Trabalhadas.xlsx
+++ b/Documentação/Horas Trabalhadas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Quantidade de horas trabalhadas no Projeto</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Procurando solução para assossiar Produtos com Grupos</t>
+  </si>
+  <si>
+    <t>Procurado e encontrado solução p/associar Produto c/Grupo</t>
+  </si>
+  <si>
+    <t>Procurando solução para assossiar Pedidos com Clientes</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,19 +572,37 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
+      <c r="A15" s="4">
+        <v>44231</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="4">
+        <v>44235</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="4">
+        <v>44236</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>

</xml_diff>